<commit_message>
Ulepszenie logowania, drobne ulepszenia dotychczasowego kodu.
</commit_message>
<xml_diff>
--- a/input/Dane klientów.xlsx
+++ b/input/Dane klientów.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="320">
   <si>
     <t xml:space="preserve">Nazwa klienta</t>
   </si>
@@ -913,15 +913,85 @@
   </si>
   <si>
     <t xml:space="preserve">ul.GRÓJECKA 132, 02-390 Warszawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.CasISZEWSKIEGO 15, 02-777 Warszawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.SIENKIEWICZA 7, 09-100 Płońsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.KSIĘDZA IGNACEGO JANA SKORUPKI 71, 05-091 Ząbki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.SIENKIEWICZA 4, 06-500 Mława</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.MIKOŁAJA KOPERNIKA 3, 06-200 Maków Mazowiecki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.GENERAŁA TADEUSZA KOŚCIUSZKI 27, 07-410 Ostrołęka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.JANA KOCHANOWSKIEGO 22A, 09-402 Płock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.BOHATERÓW MODLINA 28, 05-100 Nowy Dwór Mazowiecki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.SZKOLNA 4, 05-304 Stanisławów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.KONSTYTUCJI 3 MAJA 17, 05-250 Radzymin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.KOŚCIELNA 9, 05-205 Wola Rasztowska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.MSZCZONOWSKA 24, 05-830 Nadarzyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.WARSZAWSKA 28, 05-480 Karczew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.KSIĘDZA SAJNY 1A, 05-530 Góra Kalwaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.TOMASZOWSKA 42/3, 26-420 Nowe Miasto Nad Pilicą</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.PIASKOWA 17A, 05-825 Grodzisk Mazowiecki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.PIASTOWSKA 48, 09-200 Sierpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.LESZNO 1, 06-300 Przasnysz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.PAPCZYŃSKIEGO 1, 96-330 Puszcza Mariańska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.PLAC KOŚCIELNY 6, 07-306 Brok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.PLAC WOLNOŚCI 3, 09-300 Żuromin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.ALEJA POKOJU 5, 26-700 Zwoleń</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul.MICKIEWICZA 2, 05-310 Kałuszyn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -997,7 +1067,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1016,6 +1086,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1043,13 +1117,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2692,17 +2766,17 @@
   </sheetPr>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E81" activeCellId="0" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4087,17 +4161,1369 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.8218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>420</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>362</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>423</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>352</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>369</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>410</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>420</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E35" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E36" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E41" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E42" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E43" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E45" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E47" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E48" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E49" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E50" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E51" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E52" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E53" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E54" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E55" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E56" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E57" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E58" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E60" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E61" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E62" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E64" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E66" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E67" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E69" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E70" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E72" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E73" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E75" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E78" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E80" s="5" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>